<commit_message>
Doan day bo sung orderAmount
</commit_message>
<xml_diff>
--- a/2.Design/Template/Thong_tin_hang_trong_kho.xlsx
+++ b/2.Design/Template/Thong_tin_hang_trong_kho.xlsx
@@ -3,24 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D57078-A92C-4517-943B-DF0F3CFE2151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6999A9-4A50-4D00-8DD5-4D5CA45C4F94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>STT</t>
   </si>
@@ -29,9 +35,6 @@
   </si>
   <si>
     <t>Tên hàng</t>
-  </si>
-  <si>
-    <t>Số lượng</t>
   </si>
   <si>
     <t>&lt;jx:forEach items="${items}" var="item" varStatus="status"&gt;</t>
@@ -87,6 +90,15 @@
   </si>
   <si>
     <t>${item.issueAmountValue}</t>
+  </si>
+  <si>
+    <t>Số lượng yêu cầu</t>
+  </si>
+  <si>
+    <t>Số lượng tồn kho</t>
+  </si>
+  <si>
+    <t>${item.orderAmountValue}</t>
   </si>
 </sst>
 </file>
@@ -497,27 +509,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="37.5703125" style="5" customWidth="1"/>
-    <col min="6" max="7" width="13.140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="5.54296875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="35" style="5" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="32.08984375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="12.08984375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="16.453125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -527,10 +541,11 @@
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
       <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
     </row>
-    <row r="2" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -540,8 +555,9 @@
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -552,27 +568,30 @@
         <v>2</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="9" t="s">
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -582,39 +601,43 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="24.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -624,11 +647,12 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>